<commit_message>
Zmiana modelu aby był uczony tylko z wygranych gier, zwiekszenie ilości gier z których model się uczy.
</commit_message>
<xml_diff>
--- a/game_results.xlsx
+++ b/game_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T118"/>
+  <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6409,6 +6409,556 @@
         </is>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>2565</v>
+      </c>
+      <c r="B119" t="n">
+        <v>10</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>19</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2</v>
+      </c>
+      <c r="F119" t="n">
+        <v>9</v>
+      </c>
+      <c r="G119" t="n">
+        <v>7</v>
+      </c>
+      <c r="H119" t="n">
+        <v>1</v>
+      </c>
+      <c r="I119" t="n">
+        <v>10.52631578947368</v>
+      </c>
+      <c r="J119" t="n">
+        <v>47.36842105263158</v>
+      </c>
+      <c r="K119" t="n">
+        <v>36.84210526315789</v>
+      </c>
+      <c r="L119" t="n">
+        <v>5.263157894736842</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>2566</v>
+      </c>
+      <c r="B120" t="n">
+        <v>10</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>17</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>8</v>
+      </c>
+      <c r="G120" t="n">
+        <v>8</v>
+      </c>
+      <c r="H120" t="n">
+        <v>1</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
+      <c r="J120" t="n">
+        <v>47.05882352941176</v>
+      </c>
+      <c r="K120" t="n">
+        <v>47.05882352941176</v>
+      </c>
+      <c r="L120" t="n">
+        <v>5.88235294117647</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>2567</v>
+      </c>
+      <c r="B121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>35</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>28</v>
+      </c>
+      <c r="G121" t="n">
+        <v>6</v>
+      </c>
+      <c r="H121" t="n">
+        <v>1</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0</v>
+      </c>
+      <c r="J121" t="n">
+        <v>80</v>
+      </c>
+      <c r="K121" t="n">
+        <v>17.14285714285714</v>
+      </c>
+      <c r="L121" t="n">
+        <v>2.857142857142857</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>2568</v>
+      </c>
+      <c r="B122" t="n">
+        <v>10</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>21</v>
+      </c>
+      <c r="E122" t="n">
+        <v>7</v>
+      </c>
+      <c r="F122" t="n">
+        <v>7</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5</v>
+      </c>
+      <c r="H122" t="n">
+        <v>2</v>
+      </c>
+      <c r="I122" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="J122" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="K122" t="n">
+        <v>23.80952380952381</v>
+      </c>
+      <c r="L122" t="n">
+        <v>9.523809523809524</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>Monte Carlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>2569</v>
+      </c>
+      <c r="B123" t="n">
+        <v>10</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>36</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" t="n">
+        <v>35</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H123" t="n">
+        <v>1</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0</v>
+      </c>
+      <c r="J123" t="n">
+        <v>97.22222222222221</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0</v>
+      </c>
+      <c r="L123" t="n">
+        <v>2.777777777777778</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>2570</v>
+      </c>
+      <c r="B124" t="n">
+        <v>10</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>42</v>
+      </c>
+      <c r="E124" t="n">
+        <v>6</v>
+      </c>
+      <c r="F124" t="n">
+        <v>26</v>
+      </c>
+      <c r="G124" t="n">
+        <v>9</v>
+      </c>
+      <c r="H124" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" t="n">
+        <v>14.28571428571428</v>
+      </c>
+      <c r="J124" t="n">
+        <v>61.90476190476191</v>
+      </c>
+      <c r="K124" t="n">
+        <v>21.42857142857143</v>
+      </c>
+      <c r="L124" t="n">
+        <v>2.380952380952381</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>2571</v>
+      </c>
+      <c r="B125" t="n">
+        <v>10</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>28</v>
+      </c>
+      <c r="E125" t="n">
+        <v>4</v>
+      </c>
+      <c r="F125" t="n">
+        <v>14</v>
+      </c>
+      <c r="G125" t="n">
+        <v>9</v>
+      </c>
+      <c r="H125" t="n">
+        <v>1</v>
+      </c>
+      <c r="I125" t="n">
+        <v>14.28571428571428</v>
+      </c>
+      <c r="J125" t="n">
+        <v>50</v>
+      </c>
+      <c r="K125" t="n">
+        <v>32.14285714285715</v>
+      </c>
+      <c r="L125" t="n">
+        <v>3.571428571428571</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>2572</v>
+      </c>
+      <c r="B126" t="n">
+        <v>10</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>41</v>
+      </c>
+      <c r="E126" t="n">
+        <v>2</v>
+      </c>
+      <c r="F126" t="n">
+        <v>32</v>
+      </c>
+      <c r="G126" t="n">
+        <v>6</v>
+      </c>
+      <c r="H126" t="n">
+        <v>1</v>
+      </c>
+      <c r="I126" t="n">
+        <v>4.878048780487805</v>
+      </c>
+      <c r="J126" t="n">
+        <v>78.04878048780488</v>
+      </c>
+      <c r="K126" t="n">
+        <v>14.63414634146341</v>
+      </c>
+      <c r="L126" t="n">
+        <v>2.439024390243902</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>Neighbour Deduction</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>2573</v>
+      </c>
+      <c r="B127" t="n">
+        <v>10</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" t="n">
+        <v>1</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" t="n">
+        <v>100</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>Monte Carlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>2574</v>
+      </c>
+      <c r="B128" t="n">
+        <v>10</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>23</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>22</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" t="n">
+        <v>95.65217391304348</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" t="n">
+        <v>4.347826086956522</v>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>2575</v>
+      </c>
+      <c r="B129" t="n">
+        <v>10</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>10x10</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>33</v>
+      </c>
+      <c r="E129" t="n">
+        <v>2</v>
+      </c>
+      <c r="F129" t="n">
+        <v>20</v>
+      </c>
+      <c r="G129" t="n">
+        <v>9</v>
+      </c>
+      <c r="H129" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" t="n">
+        <v>6.060606060606061</v>
+      </c>
+      <c r="J129" t="n">
+        <v>60.60606060606061</v>
+      </c>
+      <c r="K129" t="n">
+        <v>27.27272727272727</v>
+      </c>
+      <c r="L129" t="n">
+        <v>6.060606060606061</v>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>Cluster Inference</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>